<commit_message>
small leetcode session, leading to another leetcode problem soon
</commit_message>
<xml_diff>
--- a/Longest Palindromic Substring/Whiteboards/Solution.xlsx
+++ b/Longest Palindromic Substring/Whiteboards/Solution.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\Longest Palindromic Substring\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F752182-EE25-4CE3-98FD-951870D0209B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF5B26A-0B11-49EF-BCE7-B9D1FB850DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sol1" sheetId="3" r:id="rId1"/>
+    <sheet name="Sol2 Abandoned Old" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,8 +35,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
   <si>
     <t>a</t>
   </si>
@@ -43,14 +66,109 @@
     <t>b</t>
   </si>
   <si>
-    <t>d</t>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>First the orange is all across 1s</t>
+  </si>
+  <si>
+    <t>Then the green is determined by comparing 2</t>
+  </si>
+  <si>
+    <t>then all the blues are done per level based on comparing start and end and checking if inbetween is palindrome</t>
+  </si>
+  <si>
+    <t>len</t>
+  </si>
+  <si>
+    <t>lo</t>
+  </si>
+  <si>
+    <t>For i 0-5</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>j&gt;=0?</t>
+  </si>
+  <si>
+    <t>k&lt;=s.len</t>
+  </si>
+  <si>
+    <t>.s@j=s@k</t>
+  </si>
+  <si>
+    <t>&amp;&amp;&amp;</t>
+  </si>
+  <si>
+    <t>extendPalindrome(s, 0, 0);</t>
+  </si>
+  <si>
+    <r>
+      <t>while</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF263238"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (j &gt;= </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF1C00CF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF263238"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> &amp;&amp; k &lt; s.length() &amp;&amp; s.charAt(j) == s.charAt(k))</t>
+    </r>
+  </si>
+  <si>
+    <t>.s@j</t>
+  </si>
+  <si>
+    <t>.s@k</t>
+  </si>
+  <si>
+    <t>lo=</t>
+  </si>
+  <si>
+    <t>maxlen=</t>
+  </si>
+  <si>
+    <t>mlen</t>
+  </si>
+  <si>
+    <t>extendPalindrome(s, 0, 1);</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,13 +176,83 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF263238"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1C00CF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFAA0D91"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -76,16 +264,52 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -397,19 +621,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CF585D-CE06-44D4-80AA-070156E711E0}">
-  <dimension ref="G7:L12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258D0A20-7AB3-4F3B-A614-BCA3729906B1}">
+  <dimension ref="D4:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="4.7109375" style="1"/>
+    <col min="1" max="6" width="4.7109375" style="1"/>
+    <col min="7" max="7" width="4.5703125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="4.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="7:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="4:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2</v>
+      </c>
+      <c r="K6" s="1">
+        <v>3</v>
+      </c>
+      <c r="L6" s="1">
+        <v>4</v>
+      </c>
+      <c r="M6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="4:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H7" s="1" t="s">
         <v>1</v>
       </c>
@@ -420,38 +671,491 @@
         <v>1</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="4:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="7:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G8" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="7:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G9" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="7:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G10" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="7:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G11" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="7:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G12" s="1" t="s">
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="str" cm="1">
+        <f t="array" ref="G8:G13">TRANSPOSE(H7:M7)</f>
+        <v>b</v>
+      </c>
+      <c r="H8" s="6">
+        <v>1</v>
+      </c>
+      <c r="I8" s="7">
+        <f>IF(I$7=H$7,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <f>IF(AND(J$7=H$7,I9),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="K8" s="3">
+        <f>IF(AND(K$7=H$7,J9),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
+        <f>IF(AND(L$7=H$7,K9),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="5">
+        <f>IF(AND(M7=H7,L9),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="4:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="str">
+        <v>a</v>
+      </c>
+      <c r="I9" s="6">
+        <v>1</v>
+      </c>
+      <c r="J9" s="7">
+        <f>IF(J$7=I$7,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <f>IF(AND(K$7=I$7,J10),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <f>IF(AND(L$7=I$7,K10),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M9" s="4">
+        <f>IF(AND(M$7=I$7,L10),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="4:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="1">
         <v>2</v>
       </c>
+      <c r="G10" s="1" t="str">
+        <v>b</v>
+      </c>
+      <c r="J10" s="6">
+        <v>1</v>
+      </c>
+      <c r="K10" s="7">
+        <f>IF(K$7=J$7,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="L10" s="2">
+        <f>IF(AND(L$7=J$7,K11),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="3">
+        <f>IF(AND(M$7=J$7,L11),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="4:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="1">
+        <v>3</v>
+      </c>
+      <c r="G11" s="1" t="str">
+        <v>b</v>
+      </c>
+      <c r="K11" s="6">
+        <v>1</v>
+      </c>
+      <c r="L11" s="7">
+        <f>IF(L$7=K$7,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <f>IF(AND(M$7=K$7,L12),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="9"/>
+    </row>
+    <row r="12" spans="4:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="1">
+        <v>4</v>
+      </c>
+      <c r="G12" s="1" t="str">
+        <v>a</v>
+      </c>
+      <c r="L12" s="6">
+        <v>1</v>
+      </c>
+      <c r="M12" s="7">
+        <f>IF(M$7=L$7,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="9"/>
+    </row>
+    <row r="13" spans="4:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="1">
+        <v>5</v>
+      </c>
+      <c r="G13" s="1" t="str">
+        <v>a</v>
+      </c>
+      <c r="M13" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E43A7942-5113-4E01-BCB8-EA0CEAF0F42A}">
+  <dimension ref="C3:AD21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="4.7109375" style="1"/>
+    <col min="7" max="7" width="4.5703125" style="1" customWidth="1"/>
+    <col min="8" max="12" width="4.7109375" style="1"/>
+    <col min="13" max="13" width="25.85546875" style="1" customWidth="1"/>
+    <col min="14" max="20" width="4.7109375" style="1"/>
+    <col min="21" max="21" width="9.5703125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="10" style="1" customWidth="1"/>
+    <col min="23" max="23" width="10.42578125" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="4.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1">
+        <v>3</v>
+      </c>
+      <c r="K3" s="1">
+        <v>4</v>
+      </c>
+      <c r="L3" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="W9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0</v>
+      </c>
+      <c r="U10" s="1">
+        <v>1</v>
+      </c>
+      <c r="V10" s="1">
+        <v>1</v>
+      </c>
+      <c r="W10" s="1">
+        <f>IF(Z10=AA10,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="X10" s="1">
+        <f>IF(SUM(U10:W10)=3,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Z10" s="1" t="str">
+        <f>HLOOKUP(R10,$G$3:$L$4,2,FALSE)</f>
+        <v>b</v>
+      </c>
+      <c r="AA10" s="1" t="str">
+        <f>HLOOKUP(S10,$G$3:$L$4,2,FALSE)</f>
+        <v>b</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="S11" s="13"/>
+      <c r="U11" s="1">
+        <v>1</v>
+      </c>
+      <c r="V11" s="1">
+        <v>1</v>
+      </c>
+      <c r="W11" s="1">
+        <f>IF(Z11=AA11,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="X11" s="1">
+        <f>IF(SUM(U11:W11)=3,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Z11" s="1" t="str">
+        <f>HLOOKUP(R11,$G$3:$L$4,2,FALSE)</f>
+        <v>b</v>
+      </c>
+      <c r="AA11" s="1" t="str">
+        <f>HLOOKUP(S11,$G$3:$L$4,2,FALSE)</f>
+        <v>b</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="U12" s="1">
+        <v>0</v>
+      </c>
+      <c r="V12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q15" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>1</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="W16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z16" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="6:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="R17" s="1">
+        <v>0</v>
+      </c>
+      <c r="S17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="6:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="6:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F19" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="6:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="6:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="W9" r:id="rId1" xr:uid="{F839B9DC-3FA2-44EE-8A1E-944F0B8DFA70}"/>
+    <hyperlink ref="Z9" r:id="rId2" xr:uid="{E9ABB2B1-D182-4840-B0DD-E7D3DEF090A4}"/>
+    <hyperlink ref="AA9" r:id="rId3" xr:uid="{337F0DFA-EA08-47BC-82B1-BC3316DDC258}"/>
+    <hyperlink ref="W16" r:id="rId4" xr:uid="{2D670E37-3FAC-463E-B0FF-2ABA2EEF487D}"/>
+    <hyperlink ref="Z16" r:id="rId5" xr:uid="{004A2273-4DF8-47FA-B477-1D36625E60DC}"/>
+    <hyperlink ref="AA16" r:id="rId6" xr:uid="{3B04A533-7291-4CBE-9EA1-B1EC01C75C68}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
completed Longest Palindromic Substring
</commit_message>
<xml_diff>
--- a/Longest Palindromic Substring/Whiteboards/Solution.xlsx
+++ b/Longest Palindromic Substring/Whiteboards/Solution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\Longest Palindromic Substring\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF5B26A-0B11-49EF-BCE7-B9D1FB850DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C30D353-EAC8-4AAA-A1E3-CDE6BC05E601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
+    <workbookView xWindow="34995" yWindow="4950" windowWidth="17130" windowHeight="8715" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
   <sheets>
     <sheet name="Sol1" sheetId="3" r:id="rId1"/>
@@ -58,12 +58,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="32">
   <si>
     <t>a</t>
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>v</t>
   </si>
   <si>
     <t>start</t>
@@ -162,6 +165,24 @@
   </si>
   <si>
     <t>extendPalindrome(s, 0, 1);</t>
+  </si>
+  <si>
+    <t>Round 1</t>
+  </si>
+  <si>
+    <t>Round 2</t>
+  </si>
+  <si>
+    <t>Round 3</t>
+  </si>
+  <si>
+    <t>Round 4</t>
+  </si>
+  <si>
+    <t>Round 5</t>
+  </si>
+  <si>
+    <t>Round 6</t>
   </si>
 </sst>
 </file>
@@ -268,7 +289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -305,6 +326,9 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -622,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258D0A20-7AB3-4F3B-A614-BCA3729906B1}">
-  <dimension ref="D4:R13"/>
+  <dimension ref="D4:V42"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:M7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AE22" sqref="AE22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -637,7 +661,7 @@
   <sheetData>
     <row r="4" spans="4:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="4:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -682,7 +706,7 @@
     </row>
     <row r="8" spans="4:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
@@ -716,7 +740,7 @@
       </c>
       <c r="Q8" s="8"/>
       <c r="R8" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="4:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -747,7 +771,7 @@
       </c>
       <c r="Q9" s="7"/>
       <c r="R9" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="4:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -774,7 +798,7 @@
       </c>
       <c r="Q10" s="2"/>
       <c r="R10" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="4:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -828,7 +852,342 @@
       <c r="Q13" s="5"/>
       <c r="R13" s="9"/>
     </row>
+    <row r="18" spans="6:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="I18" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" s="14"/>
+      <c r="L18" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M18" s="14"/>
+      <c r="O18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P18" s="14"/>
+      <c r="R18" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="S18" s="14"/>
+      <c r="U18" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="V18" s="14"/>
+    </row>
+    <row r="19" spans="6:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="6:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
+        <v>1</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
+        <v>2</v>
+      </c>
+      <c r="O20" s="1">
+        <v>0</v>
+      </c>
+      <c r="P20" s="1">
+        <v>3</v>
+      </c>
+      <c r="R20" s="1">
+        <v>0</v>
+      </c>
+      <c r="S20" s="1">
+        <v>4</v>
+      </c>
+      <c r="U20" s="1">
+        <v>0</v>
+      </c>
+      <c r="V20" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="6:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+      <c r="I21" s="1">
+        <v>1</v>
+      </c>
+      <c r="J21" s="1">
+        <v>2</v>
+      </c>
+      <c r="L21" s="1">
+        <v>1</v>
+      </c>
+      <c r="M21" s="1">
+        <v>3</v>
+      </c>
+      <c r="O21" s="1">
+        <v>1</v>
+      </c>
+      <c r="P21" s="1">
+        <v>4</v>
+      </c>
+      <c r="R21" s="1">
+        <v>1</v>
+      </c>
+      <c r="S21" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="6:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>2</v>
+      </c>
+      <c r="I22" s="1">
+        <v>2</v>
+      </c>
+      <c r="J22" s="1">
+        <v>3</v>
+      </c>
+      <c r="L22" s="1">
+        <v>2</v>
+      </c>
+      <c r="M22" s="1">
+        <v>4</v>
+      </c>
+      <c r="O22" s="1">
+        <v>2</v>
+      </c>
+      <c r="P22" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="6:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="1">
+        <v>3</v>
+      </c>
+      <c r="G23" s="1">
+        <v>3</v>
+      </c>
+      <c r="I23" s="1">
+        <v>3</v>
+      </c>
+      <c r="J23" s="1">
+        <v>4</v>
+      </c>
+      <c r="L23" s="1">
+        <v>3</v>
+      </c>
+      <c r="M23" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="6:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="1">
+        <v>4</v>
+      </c>
+      <c r="G24" s="1">
+        <v>4</v>
+      </c>
+      <c r="I24" s="1">
+        <v>4</v>
+      </c>
+      <c r="J24" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="6:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F25" s="1">
+        <v>5</v>
+      </c>
+      <c r="G25" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="6:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J35" s="1">
+        <v>0</v>
+      </c>
+      <c r="K35" s="1">
+        <v>1</v>
+      </c>
+      <c r="L35" s="1">
+        <v>2</v>
+      </c>
+      <c r="M35" s="1">
+        <v>3</v>
+      </c>
+      <c r="N35" s="1">
+        <v>4</v>
+      </c>
+      <c r="O35" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="6:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="6:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0</v>
+      </c>
+      <c r="I37" s="1" t="str" cm="1">
+        <f t="array" ref="I37:I42">TRANSPOSE(J36:O36)</f>
+        <v>a</v>
+      </c>
+      <c r="J37" s="6">
+        <v>1</v>
+      </c>
+      <c r="K37" s="7"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="5"/>
+    </row>
+    <row r="38" spans="6:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H38" s="1">
+        <v>1</v>
+      </c>
+      <c r="I38" s="1" t="str">
+        <v>b</v>
+      </c>
+      <c r="K38" s="6">
+        <v>1</v>
+      </c>
+      <c r="L38" s="7"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="4"/>
+    </row>
+    <row r="39" spans="6:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H39" s="1">
+        <v>2</v>
+      </c>
+      <c r="I39" s="1" t="str">
+        <v>v</v>
+      </c>
+      <c r="L39" s="6">
+        <v>1</v>
+      </c>
+      <c r="M39" s="7"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="3"/>
+    </row>
+    <row r="40" spans="6:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="1">
+        <v>3</v>
+      </c>
+      <c r="I40" s="1" t="str">
+        <v>b</v>
+      </c>
+      <c r="M40" s="6">
+        <v>1</v>
+      </c>
+      <c r="N40" s="7"/>
+      <c r="O40" s="2"/>
+    </row>
+    <row r="41" spans="6:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H41" s="1">
+        <v>4</v>
+      </c>
+      <c r="I41" s="1" t="str">
+        <v>v</v>
+      </c>
+      <c r="N41" s="6">
+        <v>1</v>
+      </c>
+      <c r="O41" s="7"/>
+    </row>
+    <row r="42" spans="6:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H42" s="1">
+        <v>5</v>
+      </c>
+      <c r="I42" s="1" t="str">
+        <v>a</v>
+      </c>
+      <c r="O42" s="6">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="U18:V18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -837,7 +1196,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E43A7942-5113-4E01-BCB8-EA0CEAF0F42A}">
   <dimension ref="C3:AD21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
@@ -876,10 +1235,10 @@
     </row>
     <row r="4" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>1</v>
@@ -902,7 +1261,7 @@
     </row>
     <row r="7" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1">
         <v>6</v>
@@ -910,53 +1269,53 @@
     </row>
     <row r="8" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="W9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="X9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q9" s="1">
-        <v>0</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="W9" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="X9" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="Z9" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AA9" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AD9" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F10" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R10" s="1">
         <v>0</v>
@@ -995,7 +1354,7 @@
     </row>
     <row r="11" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F11" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="S11" s="13"/>
       <c r="U11" s="1">
@@ -1029,7 +1388,7 @@
     </row>
     <row r="12" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F12" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U12" s="1">
         <v>0</v>
@@ -1046,7 +1405,7 @@
     </row>
     <row r="13" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F13" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>
@@ -1060,7 +1419,7 @@
     </row>
     <row r="14" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F14" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H14" s="1">
         <v>3</v>
@@ -1074,50 +1433,50 @@
     </row>
     <row r="15" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q15" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="3:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E16" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>1</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="W16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA16" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Q16" s="1">
-        <v>1</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="S16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="U16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="W16" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="X16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z16" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA16" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="AC16" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="AD16" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="6:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F17" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R17" s="1">
         <v>0</v>
@@ -1128,22 +1487,22 @@
     </row>
     <row r="18" spans="6:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F18" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="6:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F19" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="6:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F20" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="6:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F21" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>